<commit_message>
fix error of wrong final formula in xls template file
</commit_message>
<xml_diff>
--- a/app/views/templates/cheo/leader.xlsx
+++ b/app/views/templates/cheo/leader.xlsx
@@ -11,9 +11,6 @@
     <sheet name="熱意- nhiet_tinh" sheetId="5" r:id="rId2"/>
     <sheet name="leader- vai_tro" sheetId="6" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="145621" calcOnSave="0"/>
 </workbook>
 </file>
@@ -1777,7 +1774,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
@@ -1827,9 +1824,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1870,9 +1864,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1917,8 +1908,11 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1926,17 +1920,14 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1969,43 +1960,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="考え方- Tu duy"/>
-      <sheetName val="熱意- Nhiet tinh"/>
-      <sheetName val="Vai trò -Chung "/>
-      <sheetName val="Vai trò -Leader"/>
-      <sheetName val="Vai trò -Manager"/>
-      <sheetName val="能力"/>
-      <sheetName val="スキル2.0"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="28">
-          <cell r="W28" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="28">
-          <cell r="X28" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2301,17 +2255,17 @@
   <dimension ref="A1:W37"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="D18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="W28" sqref="W28"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="5.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="78.85546875" style="24" customWidth="1"/>
+    <col min="3" max="3" width="78.85546875" style="23" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="3"/>
     <col min="5" max="5" width="8.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.140625" style="3" customWidth="1"/>
@@ -2336,55 +2290,55 @@
     </row>
     <row r="2" spans="1:23" s="6" customFormat="1" ht="90">
       <c r="C2" s="7"/>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="N2" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="O2" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="P2" s="40" t="s">
+      <c r="P2" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="Q2" s="40" t="s">
+      <c r="Q2" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="R2" s="40" t="s">
+      <c r="R2" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="S2" s="40" t="s">
+      <c r="S2" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="T2" s="40" t="s">
+      <c r="T2" s="38" t="s">
         <v>132</v>
       </c>
       <c r="U2" s="8" t="s">
@@ -2405,21 +2359,22 @@
         <v>5</v>
       </c>
       <c r="D3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
       <c r="U3" s="14" t="e">
         <f t="shared" ref="U3:U27" si="0">AVERAGE(D3:T3)</f>
         <v>#DIV/0!</v>
@@ -2440,21 +2395,22 @@
         <v>6</v>
       </c>
       <c r="D4" s="12"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
       <c r="U4" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2475,21 +2431,22 @@
         <v>7</v>
       </c>
       <c r="D5" s="12"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
       <c r="U5" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2513,21 +2470,22 @@
         <v>9</v>
       </c>
       <c r="D6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
       <c r="U6" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2551,21 +2509,22 @@
         <v>11</v>
       </c>
       <c r="D7" s="12"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
       <c r="U7" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2586,21 +2545,22 @@
         <v>12</v>
       </c>
       <c r="D8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
       <c r="U8" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2624,21 +2584,22 @@
         <v>13</v>
       </c>
       <c r="D9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
       <c r="U9" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2659,21 +2620,22 @@
         <v>14</v>
       </c>
       <c r="D10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
       <c r="U10" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2694,21 +2656,22 @@
         <v>15</v>
       </c>
       <c r="D11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
       <c r="U11" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2732,21 +2695,22 @@
         <v>17</v>
       </c>
       <c r="D12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
       <c r="U12" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2767,21 +2731,22 @@
         <v>18</v>
       </c>
       <c r="D13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
       <c r="U13" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2802,21 +2767,22 @@
         <v>19</v>
       </c>
       <c r="D14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
       <c r="U14" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2837,21 +2803,22 @@
         <v>20</v>
       </c>
       <c r="D15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
       <c r="U15" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2872,21 +2839,22 @@
         <v>21</v>
       </c>
       <c r="D16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
       <c r="U16" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2910,21 +2878,22 @@
         <v>23</v>
       </c>
       <c r="D17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
       <c r="U17" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2945,21 +2914,22 @@
         <v>24</v>
       </c>
       <c r="D18" s="12"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
       <c r="U18" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -2980,21 +2950,22 @@
         <v>25</v>
       </c>
       <c r="D19" s="12"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
       <c r="U19" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3015,21 +2986,22 @@
         <v>26</v>
       </c>
       <c r="D20" s="12"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
       <c r="U20" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3053,21 +3025,22 @@
         <v>27</v>
       </c>
       <c r="D21" s="12"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
       <c r="U21" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3088,21 +3061,22 @@
         <v>28</v>
       </c>
       <c r="D22" s="12"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
       <c r="U22" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3123,21 +3097,22 @@
         <v>29</v>
       </c>
       <c r="D23" s="12"/>
-      <c r="F23" s="17"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
       <c r="U23" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3158,6 +3133,22 @@
         <v>30</v>
       </c>
       <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
       <c r="U24" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3178,6 +3169,22 @@
         <v>31</v>
       </c>
       <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
       <c r="U25" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3198,6 +3205,22 @@
         <v>32</v>
       </c>
       <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
       <c r="U26" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3218,6 +3241,22 @@
         <v>33</v>
       </c>
       <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
       <c r="U27" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3231,10 +3270,10 @@
       </c>
     </row>
     <row r="28" spans="1:23">
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="46"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="3">
         <f>SUM(D3:D27)</f>
         <v>0</v>
@@ -3303,82 +3342,82 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W28" s="18" t="e">
+      <c r="W28" s="17" t="e">
         <f>SUM(W3:W27)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="36">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C30" s="20" t="s">
+      <c r="C30" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="21"/>
+      <c r="D30" s="20"/>
     </row>
     <row r="31" spans="1:23" ht="24">
       <c r="B31" s="10">
         <v>5</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="23"/>
+      <c r="D31" s="22"/>
     </row>
     <row r="32" spans="1:23" ht="27" customHeight="1">
       <c r="B32" s="10">
         <v>4</v>
       </c>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="23"/>
+      <c r="D32" s="22"/>
     </row>
     <row r="33" spans="2:4" ht="24">
       <c r="B33" s="10">
         <v>2</v>
       </c>
-      <c r="C33" s="22" t="s">
+      <c r="C33" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D33" s="23"/>
+      <c r="D33" s="22"/>
     </row>
     <row r="34" spans="2:4" ht="24">
       <c r="B34" s="10">
         <v>0</v>
       </c>
-      <c r="C34" s="22" t="s">
+      <c r="C34" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="23"/>
+      <c r="D34" s="22"/>
     </row>
     <row r="35" spans="2:4" ht="24">
       <c r="B35" s="10">
         <v>-2</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="23"/>
+      <c r="D35" s="22"/>
     </row>
     <row r="36" spans="2:4" ht="24">
       <c r="B36" s="10">
         <v>-5</v>
       </c>
-      <c r="C36" s="22" t="s">
+      <c r="C36" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="23"/>
+      <c r="D36" s="22"/>
     </row>
     <row r="37" spans="2:4" ht="24">
       <c r="B37" s="10">
         <v>-10</v>
       </c>
-      <c r="C37" s="22" t="s">
+      <c r="C37" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D37" s="23"/>
+      <c r="D37" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3396,18 +3435,18 @@
   </sheetPr>
   <dimension ref="A1:Y36"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E2" sqref="E2:U2"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3:U27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
     <col min="2" max="2" width="19.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="45.5703125" style="27" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" style="26" customWidth="1"/>
     <col min="4" max="4" width="12.140625" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="3"/>
     <col min="6" max="6" width="8.85546875" style="3" customWidth="1"/>
@@ -3424,7 +3463,7 @@
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>45</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -3435,55 +3474,55 @@
     </row>
     <row r="2" spans="1:24" s="6" customFormat="1" ht="90">
       <c r="C2" s="7"/>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="38" t="s">
         <v>121</v>
       </c>
-      <c r="K2" s="40" t="s">
+      <c r="K2" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="40" t="s">
+      <c r="N2" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="O2" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="P2" s="40" t="s">
+      <c r="P2" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="Q2" s="40" t="s">
+      <c r="Q2" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="R2" s="40" t="s">
+      <c r="R2" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="S2" s="40" t="s">
+      <c r="S2" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="T2" s="40" t="s">
+      <c r="T2" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="U2" s="40" t="s">
+      <c r="U2" s="38" t="s">
         <v>132</v>
       </c>
       <c r="V2" s="8" t="s">
@@ -3500,29 +3539,30 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="53"/>
+      <c r="D3" s="46"/>
       <c r="E3" s="12"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
       <c r="V3" s="14" t="e">
         <f>AVERAGE(E3:U3)</f>
         <v>#DIV/0!</v>
@@ -3539,29 +3579,30 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="52" t="s">
+      <c r="C4" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="D4" s="53"/>
+      <c r="D4" s="46"/>
       <c r="E4" s="12"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
+      <c r="U4" s="12"/>
       <c r="V4" s="14" t="e">
         <f t="shared" ref="V4:V27" si="0">AVERAGE(E4:U4)</f>
         <v>#DIV/0!</v>
@@ -3578,29 +3619,30 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="53"/>
+      <c r="D5" s="46"/>
       <c r="E5" s="12"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
       <c r="V5" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3617,29 +3659,30 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="48" t="s">
+      <c r="C6" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="48"/>
       <c r="E6" s="12"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="12"/>
+      <c r="U6" s="12"/>
       <c r="V6" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3656,29 +3699,30 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="52" t="s">
+      <c r="C7" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="53"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="12"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
       <c r="V7" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3695,29 +3739,30 @@
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="52" t="s">
+      <c r="C8" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="53"/>
+      <c r="D8" s="46"/>
       <c r="E8" s="12"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="13"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+      <c r="S8" s="12"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
       <c r="V8" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3734,29 +3779,30 @@
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="49"/>
+      <c r="D9" s="48"/>
       <c r="E9" s="12"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+      <c r="S9" s="12"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
       <c r="V9" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3773,29 +3819,30 @@
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="52" t="s">
+      <c r="C10" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="53"/>
+      <c r="D10" s="46"/>
       <c r="E10" s="12"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
       <c r="V10" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3812,29 +3859,30 @@
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="52" t="s">
+      <c r="C11" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="53"/>
+      <c r="D11" s="46"/>
       <c r="E11" s="12"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
       <c r="V11" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3851,29 +3899,30 @@
       <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="52" t="s">
+      <c r="C12" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="53"/>
+      <c r="D12" s="46"/>
       <c r="E12" s="12"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" s="12"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
       <c r="V12" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3890,29 +3939,30 @@
       <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="52" t="s">
+      <c r="C13" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="53"/>
+      <c r="D13" s="46"/>
       <c r="E13" s="12"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
       <c r="V13" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3929,29 +3979,30 @@
       <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C14" s="52" t="s">
+      <c r="C14" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="53"/>
+      <c r="D14" s="46"/>
       <c r="E14" s="12"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
       <c r="V14" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -3968,29 +4019,30 @@
       <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="52" t="s">
+      <c r="C15" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="53"/>
+      <c r="D15" s="46"/>
       <c r="E15" s="12"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
-      <c r="I15" s="13"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="13"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
       <c r="V15" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4007,29 +4059,30 @@
       <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C16" s="52" t="s">
+      <c r="C16" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="53"/>
+      <c r="D16" s="46"/>
       <c r="E16" s="12"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
       <c r="V16" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4046,29 +4099,30 @@
       <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="52" t="s">
+      <c r="C17" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="53"/>
+      <c r="D17" s="46"/>
       <c r="E17" s="12"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
       <c r="V17" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4085,29 +4139,30 @@
       <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="52" t="s">
+      <c r="C18" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="D18" s="53"/>
+      <c r="D18" s="46"/>
       <c r="E18" s="12"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
       <c r="V18" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4124,29 +4179,30 @@
       <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="53"/>
+      <c r="D19" s="46"/>
       <c r="E19" s="12"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
       <c r="V19" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4163,29 +4219,30 @@
       <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="52" t="s">
+      <c r="C20" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="53"/>
+      <c r="D20" s="46"/>
       <c r="E20" s="12"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
       <c r="V20" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4202,29 +4259,30 @@
       <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="52" t="s">
+      <c r="C21" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="D21" s="53"/>
+      <c r="D21" s="46"/>
       <c r="E21" s="12"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
       <c r="V21" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4241,29 +4299,30 @@
       <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C22" s="52" t="s">
+      <c r="C22" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="53"/>
+      <c r="D22" s="46"/>
       <c r="E22" s="12"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="13"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
       <c r="V22" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4280,29 +4339,30 @@
       <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="53"/>
+      <c r="D23" s="46"/>
       <c r="E23" s="12"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="17"/>
-      <c r="U23" s="17"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
       <c r="V23" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4319,14 +4379,30 @@
       <c r="A24" s="3">
         <v>22</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="48" t="s">
+      <c r="C24" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="D24" s="49"/>
+      <c r="D24" s="48"/>
       <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="12"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="12"/>
+      <c r="N24" s="12"/>
+      <c r="O24" s="12"/>
+      <c r="P24" s="12"/>
+      <c r="Q24" s="12"/>
+      <c r="R24" s="12"/>
+      <c r="S24" s="12"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="12"/>
       <c r="V24" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4343,14 +4419,30 @@
       <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="D25" s="49"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+      <c r="U25" s="12"/>
       <c r="V25" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4367,14 +4459,30 @@
       <c r="A26" s="3">
         <v>24</v>
       </c>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="52" t="s">
+      <c r="C26" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="53"/>
+      <c r="D26" s="46"/>
       <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
+      <c r="J26" s="12"/>
+      <c r="K26" s="12"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+      <c r="U26" s="12"/>
       <c r="V26" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4391,14 +4499,30 @@
       <c r="A27" s="3">
         <v>25</v>
       </c>
-      <c r="B27" s="26" t="s">
+      <c r="B27" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="48" t="s">
+      <c r="C27" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="D27" s="49"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="S27" s="12"/>
+      <c r="T27" s="12"/>
+      <c r="U27" s="12"/>
       <c r="V27" s="14" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
@@ -4412,11 +4536,11 @@
       </c>
     </row>
     <row r="28" spans="1:24">
-      <c r="B28" s="46" t="s">
+      <c r="B28" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C28" s="46"/>
-      <c r="D28" s="46"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
       <c r="E28" s="3">
         <f>SUM(E3:E27)</f>
         <v>0</v>
@@ -4486,20 +4610,20 @@
         <v>0</v>
       </c>
       <c r="V28" s="5"/>
-      <c r="X28" s="18" t="e">
+      <c r="X28" s="17" t="e">
         <f>SUM(X3:X27)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="30" spans="1:24" ht="24">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="18" t="s">
         <v>35</v>
       </c>
       <c r="C30" s="50" t="s">
         <v>76</v>
       </c>
       <c r="D30" s="50"/>
-      <c r="E30" s="21"/>
+      <c r="E30" s="20"/>
     </row>
     <row r="31" spans="1:24" ht="51.75" customHeight="1">
       <c r="B31" s="10">
@@ -4509,60 +4633,81 @@
         <v>77</v>
       </c>
       <c r="D31" s="51"/>
-      <c r="E31" s="23"/>
+      <c r="E31" s="22"/>
     </row>
     <row r="32" spans="1:24" ht="33.75" customHeight="1">
       <c r="B32" s="10">
         <v>4</v>
       </c>
-      <c r="C32" s="47" t="s">
+      <c r="C32" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="D32" s="47"/>
-      <c r="E32" s="23"/>
+      <c r="D32" s="49"/>
+      <c r="E32" s="22"/>
     </row>
     <row r="33" spans="2:5" ht="30" customHeight="1">
       <c r="B33" s="10">
         <v>3</v>
       </c>
-      <c r="C33" s="47" t="s">
+      <c r="C33" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="D33" s="47"/>
-      <c r="E33" s="23"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="22"/>
     </row>
     <row r="34" spans="2:5" ht="31.5" customHeight="1">
       <c r="B34" s="10">
         <v>2</v>
       </c>
-      <c r="C34" s="47" t="s">
+      <c r="C34" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="D34" s="47"/>
-      <c r="E34" s="23"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="22"/>
     </row>
     <row r="35" spans="2:5" ht="39" customHeight="1">
       <c r="B35" s="10">
         <v>1</v>
       </c>
-      <c r="C35" s="47" t="s">
+      <c r="C35" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="47"/>
-      <c r="E35" s="23"/>
+      <c r="D35" s="49"/>
+      <c r="E35" s="22"/>
     </row>
     <row r="36" spans="2:5" ht="36.75" customHeight="1">
       <c r="B36" s="10">
         <v>0</v>
       </c>
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="D36" s="47"/>
-      <c r="E36" s="23"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="C36:D36"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C33:D33"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
@@ -4575,27 +4720,6 @@
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="78" orientation="portrait" r:id="rId1"/>
@@ -4610,17 +4734,17 @@
   <dimension ref="A1:Y32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
+      <selection pane="bottomRight" activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.7109375" style="3" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="3"/>
-    <col min="3" max="3" width="5.42578125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" style="27" customWidth="1"/>
     <col min="4" max="4" width="83.28515625" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="3" customWidth="1"/>
@@ -4637,7 +4761,7 @@
       <c r="A1" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="28" t="s">
         <v>84</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -4645,1082 +4769,1082 @@
       </c>
     </row>
     <row r="2" spans="1:25" ht="94.5">
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="36" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="N2" s="33" t="s">
+      <c r="N2" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="O2" s="33" t="s">
+      <c r="O2" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="P2" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="Q2" s="33" t="s">
+      <c r="Q2" s="31" t="s">
         <v>128</v>
       </c>
-      <c r="R2" s="33" t="s">
+      <c r="R2" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="S2" s="33" t="s">
+      <c r="S2" s="31" t="s">
         <v>130</v>
       </c>
-      <c r="T2" s="33" t="s">
+      <c r="T2" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="U2" s="33" t="s">
+      <c r="U2" s="31" t="s">
         <v>132</v>
       </c>
-      <c r="V2" s="44" t="s">
+      <c r="V2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="45" t="s">
+      <c r="W2" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="45" t="s">
+      <c r="X2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="45" t="s">
+      <c r="Y2" s="43" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:25" s="13" customFormat="1" ht="15.75">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="30">
         <v>1</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="42"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39" t="e">
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="37" t="e">
         <f>AVERAGE(E3:U3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="W3" s="39">
+      <c r="W3" s="37">
         <v>2</v>
       </c>
-      <c r="X3" s="39" t="e">
+      <c r="X3" s="37" t="e">
         <f>V3*W3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y3" s="43" t="e">
+      <c r="Y3" s="41" t="e">
         <f>SUM(X23, '熱意- nhiet_tinh'!X28,'考え方- tu_duy'!W28)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:25" s="13" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="31">
+      <c r="C4" s="30">
         <v>2</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="30" t="s">
         <v>88</v>
       </c>
-      <c r="E4" s="32"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="39"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39" t="e">
+      <c r="E4" s="40"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
+      <c r="K4" s="40"/>
+      <c r="L4" s="40"/>
+      <c r="M4" s="40"/>
+      <c r="N4" s="40"/>
+      <c r="O4" s="40"/>
+      <c r="P4" s="40"/>
+      <c r="Q4" s="40"/>
+      <c r="R4" s="40"/>
+      <c r="S4" s="40"/>
+      <c r="T4" s="40"/>
+      <c r="U4" s="40"/>
+      <c r="V4" s="37" t="e">
         <f t="shared" ref="V4:V22" si="0">AVERAGE(E4:U4)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="W4" s="39">
+      <c r="W4" s="37">
         <v>2</v>
       </c>
-      <c r="X4" s="39" t="e">
+      <c r="X4" s="37" t="e">
         <f t="shared" ref="X4:X22" si="1">V4*W4</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="13" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>3</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="31" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="39"/>
-      <c r="V5" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W5" s="39">
+      <c r="E5" s="40"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
+      <c r="K5" s="40"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="40"/>
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="40"/>
+      <c r="Q5" s="40"/>
+      <c r="R5" s="40"/>
+      <c r="S5" s="40"/>
+      <c r="T5" s="40"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W5" s="37">
         <v>2</v>
       </c>
-      <c r="X5" s="39" t="e">
+      <c r="X5" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:25" s="13" customFormat="1" ht="31.5">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="30">
         <v>4</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="31" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="32"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="39"/>
-      <c r="V6" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W6" s="39">
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
+      <c r="Q6" s="40"/>
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W6" s="37">
         <v>2</v>
       </c>
-      <c r="X6" s="39" t="e">
+      <c r="X6" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="7" spans="1:25" s="13" customFormat="1" ht="31.5">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="30">
         <v>5</v>
       </c>
-      <c r="D7" s="33" t="s">
+      <c r="D7" s="31" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="32"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="39"/>
-      <c r="V7" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W7" s="39">
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="40"/>
+      <c r="N7" s="40"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="40"/>
+      <c r="Q7" s="40"/>
+      <c r="R7" s="40"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="40"/>
+      <c r="U7" s="40"/>
+      <c r="V7" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W7" s="37">
         <v>2</v>
       </c>
-      <c r="X7" s="39" t="e">
+      <c r="X7" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="8" spans="1:25" s="13" customFormat="1" ht="31.5">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="30">
         <v>6</v>
       </c>
-      <c r="D8" s="33" t="s">
+      <c r="D8" s="31" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="39"/>
-      <c r="U8" s="39"/>
-      <c r="V8" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W8" s="39">
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="40"/>
+      <c r="N8" s="40"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="40"/>
+      <c r="Q8" s="40"/>
+      <c r="R8" s="40"/>
+      <c r="S8" s="40"/>
+      <c r="T8" s="40"/>
+      <c r="U8" s="40"/>
+      <c r="V8" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W8" s="37">
         <v>2</v>
       </c>
-      <c r="X8" s="39" t="e">
+      <c r="X8" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="9" spans="1:25" s="13" customFormat="1" ht="24.95" customHeight="1">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="30">
         <v>7</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="39"/>
-      <c r="V9" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W9" s="39">
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
+      <c r="T9" s="40"/>
+      <c r="U9" s="40"/>
+      <c r="V9" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W9" s="37">
         <v>2</v>
       </c>
-      <c r="X9" s="39" t="e">
+      <c r="X9" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="10" spans="1:25" s="13" customFormat="1" ht="15.75">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C10" s="31">
+      <c r="C10" s="30">
         <v>8</v>
       </c>
-      <c r="D10" s="31" t="s">
+      <c r="D10" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="E10" s="32"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="39"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="39"/>
-      <c r="V10" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W10" s="39">
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
+      <c r="K10" s="40"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="40"/>
+      <c r="N10" s="40"/>
+      <c r="O10" s="40"/>
+      <c r="P10" s="40"/>
+      <c r="Q10" s="40"/>
+      <c r="R10" s="40"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="40"/>
+      <c r="U10" s="40"/>
+      <c r="V10" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W10" s="37">
         <v>2</v>
       </c>
-      <c r="X10" s="39" t="e">
+      <c r="X10" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="11" spans="1:25" s="13" customFormat="1" ht="31.5">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="30">
         <v>9</v>
       </c>
-      <c r="D11" s="33" t="s">
+      <c r="D11" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="32"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="39"/>
-      <c r="Q11" s="39"/>
-      <c r="R11" s="39"/>
-      <c r="S11" s="39"/>
-      <c r="T11" s="39"/>
-      <c r="U11" s="39"/>
-      <c r="V11" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W11" s="39">
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
+      <c r="K11" s="40"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="40"/>
+      <c r="N11" s="40"/>
+      <c r="O11" s="40"/>
+      <c r="P11" s="40"/>
+      <c r="Q11" s="40"/>
+      <c r="R11" s="40"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="40"/>
+      <c r="U11" s="40"/>
+      <c r="V11" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W11" s="37">
         <v>2</v>
       </c>
-      <c r="X11" s="39" t="e">
+      <c r="X11" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="12" spans="1:25" s="13" customFormat="1" ht="31.5">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C12" s="31">
+      <c r="C12" s="30">
         <v>10</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="39"/>
-      <c r="Q12" s="39"/>
-      <c r="R12" s="39"/>
-      <c r="S12" s="39"/>
-      <c r="T12" s="39"/>
-      <c r="U12" s="39"/>
-      <c r="V12" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W12" s="39">
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
+      <c r="K12" s="40"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="40"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="40"/>
+      <c r="P12" s="40"/>
+      <c r="Q12" s="40"/>
+      <c r="R12" s="40"/>
+      <c r="S12" s="40"/>
+      <c r="T12" s="40"/>
+      <c r="U12" s="40"/>
+      <c r="V12" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W12" s="37">
         <v>2</v>
       </c>
-      <c r="X12" s="39" t="e">
+      <c r="X12" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="13" spans="1:25" s="13" customFormat="1" ht="31.5">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="31">
+      <c r="C13" s="30">
         <v>11</v>
       </c>
-      <c r="D13" s="33" t="s">
+      <c r="D13" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="39"/>
-      <c r="Q13" s="39"/>
-      <c r="R13" s="39"/>
-      <c r="S13" s="39"/>
-      <c r="T13" s="39"/>
-      <c r="U13" s="39"/>
-      <c r="V13" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W13" s="39">
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
+      <c r="K13" s="40"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="40"/>
+      <c r="N13" s="40"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="40"/>
+      <c r="Q13" s="40"/>
+      <c r="R13" s="40"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="40"/>
+      <c r="U13" s="40"/>
+      <c r="V13" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W13" s="37">
         <v>2</v>
       </c>
-      <c r="X13" s="39" t="e">
+      <c r="X13" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="14" spans="1:25" s="13" customFormat="1" ht="31.5">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B14" s="31" t="s">
+      <c r="B14" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C14" s="31">
+      <c r="C14" s="30">
         <v>12</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="39"/>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
-      <c r="T14" s="39"/>
-      <c r="U14" s="39"/>
-      <c r="V14" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W14" s="39">
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W14" s="37">
         <v>2</v>
       </c>
-      <c r="X14" s="39" t="e">
+      <c r="X14" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="15" spans="1:25" s="13" customFormat="1" ht="15.75">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C15" s="31">
+      <c r="C15" s="30">
         <v>13</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="30" t="s">
         <v>99</v>
       </c>
-      <c r="E15" s="32"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
-      <c r="P15" s="39"/>
-      <c r="Q15" s="39"/>
-      <c r="R15" s="39"/>
-      <c r="S15" s="39"/>
-      <c r="T15" s="39"/>
-      <c r="U15" s="39"/>
-      <c r="V15" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W15" s="39">
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+      <c r="K15" s="40"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
+      <c r="N15" s="40"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="40"/>
+      <c r="Q15" s="40"/>
+      <c r="R15" s="40"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="40"/>
+      <c r="U15" s="40"/>
+      <c r="V15" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W15" s="37">
         <v>2</v>
       </c>
-      <c r="X15" s="39" t="e">
+      <c r="X15" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="16" spans="1:25" s="13" customFormat="1" ht="31.5">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B16" s="31" t="s">
+      <c r="B16" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C16" s="31">
+      <c r="C16" s="30">
         <v>14</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
-      <c r="P16" s="39"/>
-      <c r="Q16" s="39"/>
-      <c r="R16" s="39"/>
-      <c r="S16" s="39"/>
-      <c r="T16" s="39"/>
-      <c r="U16" s="39"/>
-      <c r="V16" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W16" s="39">
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
+      <c r="K16" s="40"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="40"/>
+      <c r="N16" s="40"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="40"/>
+      <c r="Q16" s="40"/>
+      <c r="R16" s="40"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="40"/>
+      <c r="U16" s="40"/>
+      <c r="V16" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W16" s="37">
         <v>2</v>
       </c>
-      <c r="X16" s="39" t="e">
+      <c r="X16" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="17" spans="1:24" s="13" customFormat="1" ht="31.5">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="31" t="s">
+      <c r="B17" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="31">
+      <c r="C17" s="30">
         <v>15</v>
       </c>
-      <c r="D17" s="33" t="s">
+      <c r="D17" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="E17" s="32"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="39"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
-      <c r="P17" s="39"/>
-      <c r="Q17" s="39"/>
-      <c r="R17" s="39"/>
-      <c r="S17" s="39"/>
-      <c r="T17" s="39"/>
-      <c r="U17" s="39"/>
-      <c r="V17" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W17" s="39">
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="40"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="40"/>
+      <c r="Q17" s="40"/>
+      <c r="R17" s="40"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="40"/>
+      <c r="U17" s="40"/>
+      <c r="V17" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W17" s="37">
         <v>2</v>
       </c>
-      <c r="X17" s="39" t="e">
+      <c r="X17" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="18" spans="1:24" s="13" customFormat="1" ht="31.5">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="31">
+      <c r="C18" s="30">
         <v>16</v>
       </c>
-      <c r="D18" s="33" t="s">
+      <c r="D18" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E18" s="32"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
-      <c r="P18" s="39"/>
-      <c r="Q18" s="39"/>
-      <c r="R18" s="39"/>
-      <c r="S18" s="39"/>
-      <c r="T18" s="39"/>
-      <c r="U18" s="39"/>
-      <c r="V18" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W18" s="39">
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
+      <c r="K18" s="40"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="40"/>
+      <c r="N18" s="40"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="40"/>
+      <c r="Q18" s="40"/>
+      <c r="R18" s="40"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="40"/>
+      <c r="U18" s="40"/>
+      <c r="V18" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W18" s="37">
         <v>2</v>
       </c>
-      <c r="X18" s="39" t="e">
+      <c r="X18" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="19" spans="1:24" s="13" customFormat="1" ht="31.5">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="31" t="s">
+      <c r="B19" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="31">
+      <c r="C19" s="30">
         <v>17</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="E19" s="32"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
-      <c r="P19" s="39"/>
-      <c r="Q19" s="39"/>
-      <c r="R19" s="39"/>
-      <c r="S19" s="39"/>
-      <c r="T19" s="39"/>
-      <c r="U19" s="39"/>
-      <c r="V19" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W19" s="39">
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W19" s="37">
         <v>2</v>
       </c>
-      <c r="X19" s="39" t="e">
+      <c r="X19" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="20" spans="1:24" s="13" customFormat="1" ht="31.5">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="31">
+      <c r="C20" s="30">
         <v>18</v>
       </c>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="32"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
-      <c r="P20" s="39"/>
-      <c r="Q20" s="39"/>
-      <c r="R20" s="39"/>
-      <c r="S20" s="39"/>
-      <c r="T20" s="39"/>
-      <c r="U20" s="39"/>
-      <c r="V20" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W20" s="39">
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W20" s="37">
         <v>2</v>
       </c>
-      <c r="X20" s="39" t="e">
+      <c r="X20" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="21" spans="1:24" s="13" customFormat="1" ht="15.75">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C21" s="31">
+      <c r="C21" s="30">
         <v>19</v>
       </c>
-      <c r="D21" s="31" t="s">
+      <c r="D21" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="E21" s="32"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="39"/>
-      <c r="R21" s="39"/>
-      <c r="S21" s="39"/>
-      <c r="T21" s="39"/>
-      <c r="U21" s="39"/>
-      <c r="V21" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W21" s="39">
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W21" s="37">
         <v>2</v>
       </c>
-      <c r="X21" s="39" t="e">
+      <c r="X21" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="22" spans="1:24" s="13" customFormat="1" ht="31.5">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="B22" s="31" t="s">
+      <c r="B22" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="31">
+      <c r="C22" s="30">
         <v>20</v>
       </c>
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="32"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="39"/>
-      <c r="R22" s="39"/>
-      <c r="S22" s="39"/>
-      <c r="T22" s="39"/>
-      <c r="U22" s="39"/>
-      <c r="V22" s="39" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="W22" s="39">
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
+      <c r="K22" s="40"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="40"/>
+      <c r="N22" s="40"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="40"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="37" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W22" s="37">
         <v>2</v>
       </c>
-      <c r="X22" s="39" t="e">
+      <c r="X22" s="37" t="e">
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="23" spans="1:24" ht="15.75">
-      <c r="B23" s="56" t="s">
+      <c r="B23" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="57"/>
-      <c r="D23" s="58"/>
-      <c r="E23" s="41">
+      <c r="C23" s="55"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="39">
         <f t="shared" ref="E23:U23" si="2">SUM(E3:E22)</f>
         <v>0</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="32">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G23" s="37">
+      <c r="G23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H23" s="37">
+      <c r="H23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I23" s="37">
+      <c r="I23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J23" s="37">
+      <c r="J23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K23" s="37">
+      <c r="K23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L23" s="37">
+      <c r="L23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M23" s="37">
+      <c r="M23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N23" s="37">
+      <c r="N23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O23" s="37">
+      <c r="O23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P23" s="37">
+      <c r="P23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q23" s="37">
+      <c r="Q23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R23" s="37">
+      <c r="R23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S23" s="37">
+      <c r="S23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T23" s="37">
+      <c r="T23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U23" s="37">
+      <c r="U23" s="35">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V23" s="37"/>
-      <c r="W23" s="37"/>
-      <c r="X23" s="37" t="e">
+      <c r="V23" s="35"/>
+      <c r="W23" s="35"/>
+      <c r="X23" s="35" t="e">
         <f>SUM(X2:X22)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="24" spans="1:24">
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="37"/>
-      <c r="M24" s="37"/>
-      <c r="N24" s="37"/>
-      <c r="O24" s="37"/>
-      <c r="P24" s="37"/>
-      <c r="Q24" s="37"/>
-      <c r="R24" s="37"/>
-      <c r="S24" s="37"/>
-      <c r="T24" s="37"/>
-      <c r="U24" s="37"/>
-      <c r="V24" s="37"/>
-      <c r="W24" s="37"/>
-      <c r="X24" s="37" t="e">
-        <f>X23+'[1]熱意- Nhiet tinh'!X28+'[1]考え方- Tu duy'!W28</f>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="35"/>
+      <c r="N24" s="35"/>
+      <c r="O24" s="35"/>
+      <c r="P24" s="35"/>
+      <c r="Q24" s="35"/>
+      <c r="R24" s="35"/>
+      <c r="S24" s="35"/>
+      <c r="T24" s="35"/>
+      <c r="U24" s="35"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="35"/>
+      <c r="X24" s="35" t="e">
+        <f>X23+'熱意- nhiet_tinh'!X28+'考え方- tu_duy'!W28</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="1:24" ht="60">
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="33" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="59" t="s">
+      <c r="C26" s="57" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="59"/>
+      <c r="D26" s="57"/>
     </row>
     <row r="27" spans="1:24" ht="31.5" customHeight="1">
-      <c r="B27" s="36">
+      <c r="B27" s="34">
         <v>5</v>
       </c>
-      <c r="C27" s="54" t="s">
+      <c r="C27" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="D27" s="55"/>
+      <c r="D27" s="53"/>
     </row>
     <row r="28" spans="1:24" ht="31.5" customHeight="1">
-      <c r="B28" s="36">
+      <c r="B28" s="34">
         <v>4</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="D28" s="55"/>
+      <c r="D28" s="53"/>
     </row>
     <row r="29" spans="1:24" ht="31.5" customHeight="1">
-      <c r="B29" s="36">
+      <c r="B29" s="34">
         <v>3</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="55"/>
+      <c r="D29" s="53"/>
     </row>
     <row r="30" spans="1:24" ht="31.5" customHeight="1">
-      <c r="B30" s="36">
+      <c r="B30" s="34">
         <v>2</v>
       </c>
-      <c r="C30" s="54" t="s">
+      <c r="C30" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="D30" s="55"/>
+      <c r="D30" s="53"/>
     </row>
     <row r="31" spans="1:24" ht="31.5" customHeight="1">
-      <c r="B31" s="36">
+      <c r="B31" s="34">
         <v>1</v>
       </c>
-      <c r="C31" s="54" t="s">
+      <c r="C31" s="52" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="55"/>
+      <c r="D31" s="53"/>
     </row>
     <row r="32" spans="1:24" ht="31.5" customHeight="1">
-      <c r="B32" s="36">
+      <c r="B32" s="34">
         <v>0</v>
       </c>
-      <c r="C32" s="54" t="s">
+      <c r="C32" s="52" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="55"/>
+      <c r="D32" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>